<commit_message>
added xl techniques and solverstudio examples
</commit_message>
<xml_diff>
--- a/xl/excel-techniques.xlsx
+++ b/xl/excel-techniques.xlsx
@@ -4,25 +4,94 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="14100" windowHeight="10110" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="13500" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
     <sheet name="choose" sheetId="1" r:id="rId2"/>
     <sheet name="tables" sheetId="3" r:id="rId3"/>
     <sheet name="TEST" sheetId="4" r:id="rId4"/>
-    <sheet name="LOG" sheetId="5" r:id="rId5"/>
+    <sheet name="LOG" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_AutomaticResultsDisplayMode" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceConfidenceLevel" hidden="1">0.95</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePercentileToTest" hidden="1">0.9</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformMeanTest" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformPercentileTest" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergencePerformStdDeviationTest" hidden="1">FALSE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTestAllOutputs" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTestingPeriod" hidden="1">100</definedName>
+    <definedName name="_AtRisk_SimSetting_ConvergenceTolerance" hidden="1">0.03</definedName>
+    <definedName name="_AtRisk_SimSetting_LiveUpdate" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_LiveUpdatePeriod" hidden="1">-1</definedName>
+    <definedName name="_AtRisk_SimSetting_RandomNumberGenerator" hidden="1">7</definedName>
+    <definedName name="_AtRisk_SimSetting_ReportsList" hidden="1">255</definedName>
+    <definedName name="_AtRisk_SimSetting_SimNameCount" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_SmartSensitivityAnalysisEnabled" hidden="1">TRUE</definedName>
+    <definedName name="_AtRisk_SimSetting_StatisticFunctionUpdating" hidden="1">1</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcBehavior" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
+    <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
+    <definedName name="_Order2" hidden="1">0</definedName>
+    <definedName name="demand.badindex" hidden="1">1</definedName>
+    <definedName name="equipment_cost_hr.badindex" hidden="1">1</definedName>
+    <definedName name="equipment_hrs_required.badindex" hidden="1">1</definedName>
+    <definedName name="equipment_hrs_required.firstindex" hidden="1">"row"</definedName>
+    <definedName name="equipments.badindex" hidden="1">1</definedName>
+    <definedName name="labor_hrs_required.badindex" hidden="1">1</definedName>
+    <definedName name="labor_hrs_required.firstindex" hidden="1">"row"</definedName>
+    <definedName name="machine_cost_hr.badindex" hidden="1">1</definedName>
+    <definedName name="machine_hrs_required.badindex" hidden="1">1</definedName>
+    <definedName name="machine_hrs_required.firstindex" hidden="1">"row"</definedName>
+    <definedName name="machines.badindex" hidden="1">1</definedName>
+    <definedName name="markup.badindex" hidden="1">1</definedName>
+    <definedName name="MATERIAL.dirn" hidden="1">"row"</definedName>
+    <definedName name="material_cost.badindex" hidden="1">1</definedName>
+    <definedName name="materials_required.badindex" hidden="1">1</definedName>
+    <definedName name="materials_required.firstindex" hidden="1">"row"</definedName>
+    <definedName name="operation.badindex" hidden="1">1</definedName>
+    <definedName name="Pal_Workbook_GUID" hidden="1">"G1VTY5UADFH6A9IKNWFKPKZ2"</definedName>
+    <definedName name="RiskAfterRecalcMacro" hidden="1">""</definedName>
+    <definedName name="RiskAfterSimMacro" hidden="1">""</definedName>
+    <definedName name="RiskBeforeRecalcMacro" hidden="1">""</definedName>
+    <definedName name="RiskBeforeSimMacro" hidden="1">""</definedName>
+    <definedName name="RiskCollectDistributionSamples" hidden="1">2</definedName>
+    <definedName name="RiskFixedSeed" hidden="1">1</definedName>
+    <definedName name="RiskHasSettings" hidden="1">5</definedName>
+    <definedName name="RiskMinimizeOnStart" hidden="1">FALSE</definedName>
+    <definedName name="RiskMonitorConvergence" hidden="1">FALSE</definedName>
+    <definedName name="RiskMultipleCPUSupportEnabled" hidden="1">TRUE</definedName>
+    <definedName name="RiskNumIterations" hidden="1">500</definedName>
+    <definedName name="RiskNumSimulations" hidden="1">1</definedName>
+    <definedName name="RiskPauseOnError" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunAfterRecalcMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunAfterSimMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunBeforeRecalcMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskRunBeforeSimMacro" hidden="1">FALSE</definedName>
+    <definedName name="RiskSamplingType" hidden="1">3</definedName>
+    <definedName name="RiskStandardRecalc" hidden="1">1</definedName>
+    <definedName name="RiskUpdateDisplay" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
+    <definedName name="RiskUseMultipleCPUs" hidden="1">TRUE</definedName>
     <definedName name="sampleA">tables!$G$2:$G$6</definedName>
     <definedName name="sampleB">tables!$H$2:$H$6</definedName>
+    <definedName name="supply.badindex" hidden="1">1</definedName>
+    <definedName name="tests">TEST!$D$9:$D$351</definedName>
+    <definedName name="work_cost_hr.badindex" hidden="1">1</definedName>
+    <definedName name="work_hrs_required.badindex" hidden="1">1</definedName>
+    <definedName name="work_hrs_required.firstindex" hidden="1">"row"</definedName>
+    <definedName name="workers.badindex" hidden="1">1</definedName>
+    <definedName name="years">{0,1,2,3,4,5,6,7,8,9,10}</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
   <si>
     <t>A</t>
   </si>
@@ -175,13 +244,82 @@
   </si>
   <si>
     <t>Array formula multiplication</t>
+  </si>
+  <si>
+    <t>number of tests passed</t>
+  </si>
+  <si>
+    <t>number of tests failed</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>test_all</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>test_contract_period</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>check project start and end date are consistent with contract period</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>add more tests</t>
+  </si>
+  <si>
+    <t>LOG</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>by</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t></t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,16 +349,71 @@
       <family val="1"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings 3"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="8"/>
+        <bgColor indexed="12"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -243,11 +436,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -273,11 +544,76 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 2 2" xfId="1"/>
+    <cellStyle name="Style 31" xfId="2"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -295,11 +631,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="dataTable" displayName="dataTable" ref="A1:E6" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="id" dataDxfId="2"/>
+    <tableColumn id="1" name="id" dataDxfId="4"/>
     <tableColumn id="2" name="name"/>
     <tableColumn id="5" name="role"/>
-    <tableColumn id="3" name="age" dataDxfId="1"/>
-    <tableColumn id="4" name="salary" dataDxfId="0"/>
+    <tableColumn id="3" name="age" dataDxfId="3"/>
+    <tableColumn id="4" name="salary" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -590,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -741,6 +1077,11 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
+    <row r="20" spans="2:5">
+      <c r="C20" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -751,7 +1092,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -841,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1077,11 +1418,11 @@
         <v>34</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="1">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="str">
         <f>INDEX(dataTable[], MATCH(B18, dataTable[[#All],[name]],0), MATCH(C18, dataTable[#Headers], 0))</f>
-        <v>500</v>
+        <v>manager</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
@@ -1158,9 +1499,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
       <formula1>$G$1:$H$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18 C21">
+      <formula1>INDIRECT("dataTable[#Headers]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1172,28 +1516,847 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="13">
+        <f>COUNTIF(tests, "=TRUE")</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="14">
+        <f>COUNTIF(tests, "=FALSE")</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="15">
+        <f>SUM(D2:D3)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="17" t="b">
+        <f>AND(tests)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="16"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="16"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="17" t="b">
+        <f>F10=H10</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="20">
+        <v>100</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="20">
+        <v>100</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="16"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="16"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D7 D10">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <sheetPr codeName="Sheet17">
+    <tabColor theme="0" tint="-0.249977111117893"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:E88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="11"/>
+    <col min="3" max="3" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="11"/>
+    <col min="5" max="5" width="70.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="27">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.79</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="31"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="31"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="31"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="31"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="31"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="31"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="31"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="31"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="31"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="31"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="B46" s="31"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="B47" s="31"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+    </row>
+    <row r="49" spans="2:5">
+      <c r="B49" s="31"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+    </row>
+    <row r="50" spans="2:5">
+      <c r="B50" s="31"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+    </row>
+    <row r="51" spans="2:5">
+      <c r="B51" s="31"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+    </row>
+    <row r="52" spans="2:5">
+      <c r="B52" s="31"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="B53" s="31"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" s="31"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="31"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="31"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" s="31"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="31"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="31"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" s="31"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" s="31"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" s="31"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+    </row>
+    <row r="63" spans="2:5">
+      <c r="B63" s="31"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+    </row>
+    <row r="64" spans="2:5">
+      <c r="B64" s="31"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="31"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+    </row>
+    <row r="66" spans="2:5">
+      <c r="B66" s="31"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+    </row>
+    <row r="67" spans="2:5">
+      <c r="B67" s="31"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="30"/>
+    </row>
+    <row r="68" spans="2:5">
+      <c r="B68" s="31"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="31"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+    </row>
+    <row r="70" spans="2:5">
+      <c r="B70" s="31"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="31"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="30"/>
+    </row>
+    <row r="72" spans="2:5">
+      <c r="B72" s="31"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="30"/>
+    </row>
+    <row r="73" spans="2:5">
+      <c r="B73" s="27"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+    </row>
+    <row r="74" spans="2:5">
+      <c r="B74" s="27"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+    </row>
+    <row r="75" spans="2:5">
+      <c r="B75" s="27"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+    </row>
+    <row r="76" spans="2:5">
+      <c r="B76" s="27"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+    </row>
+    <row r="77" spans="2:5">
+      <c r="B77" s="27"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+    </row>
+    <row r="78" spans="2:5">
+      <c r="B78" s="27"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="30"/>
+    </row>
+    <row r="79" spans="2:5">
+      <c r="B79" s="27"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+    </row>
+    <row r="80" spans="2:5">
+      <c r="B80" s="27"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="30"/>
+    </row>
+    <row r="81" spans="2:5">
+      <c r="B81" s="31"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82" s="31"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="30"/>
+    </row>
+    <row r="83" spans="2:5">
+      <c r="B83" s="31"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="30"/>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84" s="31"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="B85" s="31"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+    </row>
+    <row r="86" spans="2:5">
+      <c r="B86" s="31"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="30"/>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="31"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+    </row>
+    <row r="88" spans="2:5">
+      <c r="B88" s="27"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="30"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added lp xlsx examples
</commit_message>
<xml_diff>
--- a/xl/excel-techniques.xlsx
+++ b/xl/excel-techniques.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="13500" windowHeight="9045"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="13500" windowHeight="9045" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="intro" sheetId="2" r:id="rId1"/>
@@ -76,8 +76,10 @@
     <definedName name="RiskUseDifferentSeedForEachSim" hidden="1">FALSE</definedName>
     <definedName name="RiskUseFixedSeed" hidden="1">FALSE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">TRUE</definedName>
+    <definedName name="role_in">tables!$C$26</definedName>
     <definedName name="sampleA">tables!$G$2:$G$6</definedName>
     <definedName name="sampleB">tables!$H$2:$H$6</definedName>
+    <definedName name="subrange">INDEX(dataTable[salary], MATCH(role_in, dataTable[role], 0)): INDEX(dataTable[salary], MATCH(role_in, dataTable[role], 1))</definedName>
     <definedName name="supply.badindex" hidden="1">1</definedName>
     <definedName name="tests">TEST!$D$9:$D$351</definedName>
     <definedName name="work_cost_hr.badindex" hidden="1">1</definedName>
@@ -91,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="78">
   <si>
     <t>A</t>
   </si>
@@ -310,6 +312,21 @@
   </si>
   <si>
     <t></t>
+  </si>
+  <si>
+    <t>role_in</t>
+  </si>
+  <si>
+    <t>(INDEX, MATCH) : (INDEX, MATCH)</t>
+  </si>
+  <si>
+    <t>subrange</t>
+  </si>
+  <si>
+    <t>SELECT WHERE using array formula</t>
+  </si>
+  <si>
+    <t>SUM IF WHERE using array formula</t>
   </si>
 </sst>
 </file>
@@ -518,7 +535,7 @@
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,6 +610,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1180,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1222,7 +1242,7 @@
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
@@ -1245,7 +1265,7 @@
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>20</v>
@@ -1470,36 +1490,111 @@
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="D25" s="10">
-        <f t="array" ref="D25:D29">dataTable[age] * dataTable[salary]</f>
+      <c r="C25" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="C26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="1">
+        <f>SUM(subrange)</f>
+        <v>920</v>
+      </c>
+      <c r="E26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="D27" s="1">
+        <f t="array" ref="D27">SUM(IF(dataTable[role]=role_in, dataTable[salary], 0))</f>
+        <v>920</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="C28" s="34"/>
+      <c r="D28" s="1">
+        <f t="array" ref="D28:D32">IF(dataTable[role]=role_in, dataTable[salary], 0)</f>
+        <v>220</v>
+      </c>
+      <c r="E28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="C29" s="34"/>
+      <c r="D29" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="C30" s="34"/>
+      <c r="D30" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="C31" s="34"/>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="C32" s="34"/>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
+      <c r="C33" s="34"/>
+    </row>
+    <row r="34" spans="3:5">
+      <c r="C34" s="34"/>
+    </row>
+    <row r="35" spans="3:5">
+      <c r="C35" s="34"/>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="C36" s="34"/>
+    </row>
+    <row r="38" spans="3:5">
+      <c r="D38" s="10">
+        <f t="array" ref="D38:D42">dataTable[age] * dataTable[salary]</f>
         <v>2200</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E38" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
-      <c r="D26" s="10">
+    <row r="39" spans="3:5">
+      <c r="D39" s="10">
         <v>4000</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
-      <c r="D27" s="10">
+    <row r="40" spans="3:5">
+      <c r="D40" s="10">
         <v>15000</v>
       </c>
     </row>
-    <row r="28" spans="2:5">
-      <c r="D28" s="10">
+    <row r="41" spans="3:5">
+      <c r="D41" s="10">
         <v>10400</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
-      <c r="D29" s="10">
+    <row r="42" spans="3:5">
+      <c r="D42" s="10">
         <v>15500</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
       <formula1>$G$1:$H$1</formula1>
     </dataValidation>

</xml_diff>